<commit_message>
Dashboard optimizations: Remove Multi-Timeframe section, increase hourly breadth to 200 stocks, document collection improvements
</commit_message>
<xml_diff>
--- a/Daily/analysis/Weekly_Reports/weekly_breakdown_summary.xlsx
+++ b/Daily/analysis/Weekly_Reports/weekly_breakdown_summary.xlsx
@@ -61,6 +61,9 @@
     <t>Week 1</t>
   </si>
   <si>
+    <t>Jul 26 - Aug 01</t>
+  </si>
+  <si>
     <t>Jul 19 - Jul 25</t>
   </si>
   <si>
@@ -70,19 +73,19 @@
     <t>Jul 05 - Jul 11</t>
   </si>
   <si>
-    <t>Jun 28 - Jul 04</t>
-  </si>
-  <si>
-    <t>FORCEMOT</t>
-  </si>
-  <si>
-    <t>SHK</t>
+    <t>JSL</t>
+  </si>
+  <si>
+    <t>SHYAMMETL</t>
+  </si>
+  <si>
+    <t>AGI</t>
   </si>
   <si>
     <t>ANANDRATHI</t>
   </si>
   <si>
-    <t>ASHAPURMIN</t>
+    <t>AARTIIND</t>
   </si>
   <si>
     <t>MRPL</t>
@@ -92,9 +95,6 @@
   </si>
   <si>
     <t>MSUMI</t>
-  </si>
-  <si>
-    <t>ASHOKLEY</t>
   </si>
 </sst>
 </file>
@@ -501,31 +501,31 @@
         <v>15</v>
       </c>
       <c r="C2">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2">
-        <v>17.77777777777778</v>
+        <v>21.73913043478261</v>
       </c>
       <c r="G2">
-        <v>-1.889939966310729</v>
+        <v>-2.504204763949144</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
       </c>
       <c r="I2">
-        <v>1.574489853919172</v>
+        <v>2.045093221563806</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
       </c>
       <c r="K2">
-        <v>-8.911339939123108</v>
+        <v>-9.508963367108338</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -536,31 +536,31 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D3">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>51</v>
       </c>
       <c r="F3">
-        <v>31.08108108108108</v>
+        <v>15</v>
       </c>
       <c r="G3">
-        <v>-2.397239677780935</v>
+        <v>-5.003652024233992</v>
       </c>
       <c r="H3" t="s">
         <v>20</v>
       </c>
       <c r="I3">
-        <v>8.83599202392822</v>
+        <v>4.643413769011655</v>
       </c>
       <c r="J3" t="s">
         <v>24</v>
       </c>
       <c r="K3">
-        <v>-11.31290725079716</v>
+        <v>-20.23832653325562</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -571,31 +571,31 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="D4">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E4">
-        <v>38</v>
+        <v>80</v>
       </c>
       <c r="F4">
-        <v>40.625</v>
+        <v>20.79207920792079</v>
       </c>
       <c r="G4">
-        <v>-1.599632806528792</v>
+        <v>-4.727910665635076</v>
       </c>
       <c r="H4" t="s">
         <v>21</v>
       </c>
       <c r="I4">
-        <v>17.74266982334729</v>
+        <v>12.16232227488151</v>
       </c>
       <c r="J4" t="s">
         <v>25</v>
       </c>
       <c r="K4">
-        <v>-33.38225701239399</v>
+        <v>-16.26923610148342</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -606,31 +606,31 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="D5">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="F5">
-        <v>31.38686131386861</v>
+        <v>33.88429752066116</v>
       </c>
       <c r="G5">
-        <v>-2.283771291934418</v>
+        <v>-3.694411749866992</v>
       </c>
       <c r="H5" t="s">
         <v>22</v>
       </c>
       <c r="I5">
-        <v>23.5214446952596</v>
+        <v>18.49389910763066</v>
       </c>
       <c r="J5" t="s">
         <v>26</v>
       </c>
       <c r="K5">
-        <v>-51.61674270977981</v>
+        <v>-38.87801696020875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>